<commit_message>
update html tables bubble chart
</commit_message>
<xml_diff>
--- a/DataFiles_Excel/Maps/AwardsByLocation/World/World_Discretionary/World_Discretionary_HHS.xlsx
+++ b/DataFiles_Excel/Maps/AwardsByLocation/World/World_Discretionary/World_Discretionary_HHS.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Engineering Projects\Annual Report\2016-html2excel\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="1520" yWindow="1240" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="World_Discretionary_HHS" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -369,141 +369,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,323 +386,39 @@
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Myriad Pro"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Myriad Pro"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Myriad Pro"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -873,145 +462,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1026,44 +537,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1091,31 +602,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1143,23 +637,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1171,200 +648,260 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="60" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-    </row>
-    <row r="3" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="8"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1375,14 +912,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16" thickBot="1">
       <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="11"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1393,7 +930,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1404,7 +941,7 @@
         <v>440000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1415,7 +952,7 @@
         <v>12330121</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1426,7 +963,7 @@
         <v>1050000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16" thickBot="1">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1437,7 +974,7 @@
         <v>1315821</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1448,7 +985,7 @@
         <v>243350</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16" thickBot="1">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1459,7 +996,7 @@
         <v>9402447</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1470,7 +1007,7 @@
         <v>550000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16" thickBot="1">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1481,7 +1018,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16" thickBot="1">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1492,7 +1029,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16" thickBot="1">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1503,7 +1040,7 @@
         <v>7964527</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="16" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1514,7 +1051,7 @@
         <v>276309</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16" thickBot="1">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1525,7 +1062,7 @@
         <v>558234</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16" thickBot="1">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1536,7 +1073,7 @@
         <v>210000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16" thickBot="1">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1547,7 +1084,7 @@
         <v>11642191</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16" thickBot="1">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1558,7 +1095,7 @@
         <v>8025250</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16" thickBot="1">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1569,7 +1106,7 @@
         <v>399999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1580,7 +1117,7 @@
         <v>1726238</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +1128,7 @@
         <v>19991081</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1602,7 +1139,7 @@
         <v>44840933</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16" thickBot="1">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1613,7 +1150,7 @@
         <v>6646515</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16" thickBot="1">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1624,7 +1161,7 @@
         <v>2211486</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16" thickBot="1">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1635,7 +1172,7 @@
         <v>2901414</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="16" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1646,7 +1183,7 @@
         <v>2239131</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="16" thickBot="1">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1657,7 +1194,7 @@
         <v>910000</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -1668,7 +1205,7 @@
         <v>2083394</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="16" thickBot="1">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -1679,7 +1216,7 @@
         <v>113331017</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16" thickBot="1">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1690,7 +1227,7 @@
         <v>6680435</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="16" thickBot="1">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -1701,7 +1238,7 @@
         <v>1256690</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="16" thickBot="1">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -1712,7 +1249,7 @@
         <v>12782529</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="16" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -1723,7 +1260,7 @@
         <v>5937665</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="16" thickBot="1">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
@@ -1734,7 +1271,7 @@
         <v>19143409</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -1745,7 +1282,7 @@
         <v>8480269</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="16" thickBot="1">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -1756,7 +1293,7 @@
         <v>2135000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="16" thickBot="1">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -1767,7 +1304,7 @@
         <v>1274400</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="16" thickBot="1">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -1778,7 +1315,7 @@
         <v>54865444</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="16" thickBot="1">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -1789,7 +1326,7 @@
         <v>1299556</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="16" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -1800,7 +1337,7 @@
         <v>1013843</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="16" thickBot="1">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -1811,7 +1348,7 @@
         <v>21502586</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="16" thickBot="1">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -1822,7 +1359,7 @@
         <v>2335769</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="16" thickBot="1">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
@@ -1833,7 +1370,7 @@
         <v>829766</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="16" thickBot="1">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -1844,7 +1381,7 @@
         <v>1319489</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="16" thickBot="1">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
@@ -1855,7 +1392,7 @@
         <v>275284</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="16" thickBot="1">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -1866,7 +1403,7 @@
         <v>29806299</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="16" thickBot="1">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -1877,7 +1414,7 @@
         <v>781761</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="16" thickBot="1">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
@@ -1888,7 +1425,7 @@
         <v>353502</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="16" thickBot="1">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -1899,7 +1436,7 @@
         <v>6279077</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="16" thickBot="1">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -1910,7 +1447,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="16" thickBot="1">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
@@ -1921,7 +1458,7 @@
         <v>140411934</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="16" thickBot="1">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -1932,7 +1469,7 @@
         <v>505110</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="16" thickBot="1">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
@@ -1943,7 +1480,7 @@
         <v>575000</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="16" thickBot="1">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
@@ -1954,7 +1491,7 @@
         <v>527363</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="16" thickBot="1">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -1965,7 +1502,7 @@
         <v>1455535</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="16" thickBot="1">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
@@ -1976,7 +1513,7 @@
         <v>399920</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="16" thickBot="1">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -1987,7 +1524,7 @@
         <v>470254</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="16" thickBot="1">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
@@ -1998,7 +1535,7 @@
         <v>14923871</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="16" thickBot="1">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -2009,7 +1546,7 @@
         <v>136728</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="16" thickBot="1">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -2020,7 +1557,7 @@
         <v>2740726</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="16" thickBot="1">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -2031,7 +1568,7 @@
         <v>6232211</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="16" thickBot="1">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -2042,7 +1579,7 @@
         <v>652872</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="16" thickBot="1">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -2053,7 +1590,7 @@
         <v>9771160</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="16" thickBot="1">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -2064,7 +1601,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="16" thickBot="1">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -2075,7 +1612,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="16" thickBot="1">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
@@ -2086,7 +1623,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="16" thickBot="1">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
@@ -2097,7 +1634,7 @@
         <v>86114831</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="16" thickBot="1">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
@@ -2108,7 +1645,7 @@
         <v>23378241</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="16" thickBot="1">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
@@ -2119,7 +1656,7 @@
         <v>119389</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="16" thickBot="1">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -2130,7 +1667,7 @@
         <v>1567616</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="16" thickBot="1">
       <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
@@ -2141,7 +1678,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="16" thickBot="1">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
@@ -2152,7 +1689,7 @@
         <v>346616</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="16" thickBot="1">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2163,7 +1700,7 @@
         <v>179127827</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="16" thickBot="1">
       <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
@@ -2174,7 +1711,7 @@
         <v>13088972</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="16" thickBot="1">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2185,7 +1722,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="16" thickBot="1">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
@@ -2196,7 +1733,7 @@
         <v>3012984</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="16" thickBot="1">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -2207,7 +1744,7 @@
         <v>7838712</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="16" thickBot="1">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
@@ -2218,7 +1755,7 @@
         <v>1153919</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="16" thickBot="1">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
@@ -2229,7 +1766,7 @@
         <v>365000</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="16" thickBot="1">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -2240,7 +1777,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="16" thickBot="1">
       <c r="A89" s="1" t="s">
         <v>86</v>
       </c>
@@ -2251,7 +1788,7 @@
         <v>5223909</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="16" thickBot="1">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -2262,7 +1799,7 @@
         <v>1207063</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="16" thickBot="1">
       <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
@@ -2273,7 +1810,7 @@
         <v>534353471</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="16" thickBot="1">
       <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
@@ -2284,7 +1821,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="16" thickBot="1">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -2295,7 +1832,7 @@
         <v>37944759</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="16" thickBot="1">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
@@ -2306,7 +1843,7 @@
         <v>3090242</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="16" thickBot="1">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -2317,7 +1854,7 @@
         <v>2564751</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="16" thickBot="1">
       <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
@@ -2328,7 +1865,7 @@
         <v>118638</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="16" thickBot="1">
       <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
@@ -2339,7 +1876,7 @@
         <v>310702038</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="16" thickBot="1">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
@@ -2350,7 +1887,7 @@
         <v>1431441</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="16" thickBot="1">
       <c r="A99" s="1" t="s">
         <v>96</v>
       </c>
@@ -2361,7 +1898,7 @@
         <v>521551</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="16" thickBot="1">
       <c r="A100" s="1" t="s">
         <v>97</v>
       </c>
@@ -2372,7 +1909,7 @@
         <v>576952</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="16" thickBot="1">
       <c r="A101" s="1" t="s">
         <v>98</v>
       </c>
@@ -2383,7 +1920,7 @@
         <v>1490342</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="16" thickBot="1">
       <c r="A102" s="1" t="s">
         <v>99</v>
       </c>
@@ -2394,7 +1931,7 @@
         <v>19613933</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="16" thickBot="1">
       <c r="A103" s="1" t="s">
         <v>100</v>
       </c>
@@ -2405,7 +1942,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="16" thickBot="1">
       <c r="A104" s="1" t="s">
         <v>101</v>
       </c>
@@ -2416,7 +1953,7 @@
         <v>146202157</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="16" thickBot="1">
       <c r="A105" s="1" t="s">
         <v>102</v>
       </c>
@@ -2427,7 +1964,7 @@
         <v>11137285</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="16" thickBot="1">
       <c r="A106" s="1" t="s">
         <v>103</v>
       </c>
@@ -2438,7 +1975,7 @@
         <v>249000</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="16" thickBot="1">
       <c r="A107" s="1" t="s">
         <v>104</v>
       </c>
@@ -2449,7 +1986,7 @@
         <v>3282936</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="16" thickBot="1">
       <c r="A108" s="1" t="s">
         <v>105</v>
       </c>
@@ -2460,7 +1997,7 @@
         <v>437642</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="16" thickBot="1">
       <c r="A109" s="1" t="s">
         <v>106</v>
       </c>
@@ -2471,7 +2008,7 @@
         <v>227152392</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="16" thickBot="1">
       <c r="A110" s="1" t="s">
         <v>107</v>
       </c>
@@ -2482,7 +2019,7 @@
         <v>6595723</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="16" thickBot="1">
       <c r="A111" s="1" t="s">
         <v>108</v>
       </c>
@@ -2493,18 +2030,18 @@
         <v>28216463</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="16" thickBot="1">
       <c r="A112" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B112" s="6">
-        <v>70294</v>
+        <v>68762</v>
       </c>
       <c r="C112" s="5">
         <v>50407050404</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" ht="16" thickBot="1">
       <c r="A113" s="1" t="s">
         <v>110</v>
       </c>
@@ -2515,7 +2052,7 @@
         <v>199355</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" ht="16" thickBot="1">
       <c r="A114" s="1" t="s">
         <v>111</v>
       </c>
@@ -2526,7 +2063,7 @@
         <v>11462842</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" ht="16" thickBot="1">
       <c r="A115" s="1" t="s">
         <v>112</v>
       </c>
@@ -2537,7 +2074,7 @@
         <v>28920972</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" ht="16" thickBot="1">
       <c r="A116" s="1" t="s">
         <v>113</v>
       </c>
@@ -2548,7 +2085,7 @@
         <v>93141984</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" ht="16" thickBot="1">
       <c r="A117" s="1" t="s">
         <v>114</v>
       </c>
@@ -2560,16 +2097,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:C3"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="C9:C10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>